<commit_message>
fix bag with js
</commit_message>
<xml_diff>
--- a/register_of_talented_students/media/export.xlsx
+++ b/register_of_talented_students/media/export.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,112 +483,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ВСОШ по физре</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Безруков Владислав Александрович</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Технология</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>9в</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Спорт</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Школьный</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Призёр</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>22.07.2021</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>26.02.2023</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>26.02.2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ВСОШ по информатике</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Жинжило Татьяна Кирилловна</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Русский язык</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>9в</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Спорт</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Школьный</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Участник</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>12.12.2012</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>26.02.2023</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>26.02.2023</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
little excel spreadsheet styling
</commit_message>
<xml_diff>
--- a/register_of_talented_students/media/export.xlsx
+++ b/register_of_talented_students/media/export.xlsx
@@ -420,6 +420,20 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">

</xml_diff>

<commit_message>
Create school classes app.
Created new school classes app. Changed folders.
</commit_message>
<xml_diff>
--- a/register_of_talented_students/media/export.xlsx
+++ b/register_of_talented_students/media/export.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
     <col width="20" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="50" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
     <col width="15" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="15" customWidth="1" min="12" max="12"/>
@@ -497,6 +497,64 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1 новость</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Краснова Ксения Максимовна</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sdfsdfsdf</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Технология</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1а</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Спорт</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Школьный</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Лауреат</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>12.02.2007</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>29.03.2023</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Try to fix bug with char 'c'. Update school classes views.
Try to fix bug with char 'c' in school_class name, with related name. Update school class list views. Update school classes services.
</commit_message>
<xml_diff>
--- a/register_of_talented_students/media/export.xlsx
+++ b/register_of_talented_students/media/export.xlsx
@@ -500,17 +500,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1 новость</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Краснова Ксения Максимовна</t>
+          <t>Гаджиев Расул Магомедович</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sdfsdfsdf</t>
+          <t>asdasdasdasd</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -520,12 +520,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1а</t>
+          <t>1в</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Спорт</t>
+          <t>Образование</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -538,20 +538,24 @@
           <t>Лауреат</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>12.02.2007</t>
+          <t>12.12.2023</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>29.03.2023</t>
+          <t>30.03.2023</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>29.03.2023</t>
+          <t>30.03.2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update school class views.
Add new template tag (add index). Update school class views. Update school class model.
</commit_message>
<xml_diff>
--- a/register_of_talented_students/media/export.xlsx
+++ b/register_of_talented_students/media/export.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,68 +497,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Гаджиев Расул Магомедович</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>asdasdasdasd</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Технология</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1в</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Образование</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Школьный</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Лауреат</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>12.12.2023</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>30.03.2023</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>30.03.2023</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>